<commit_message>
added sample code for encrypting files
</commit_message>
<xml_diff>
--- a/Time Sheet/Patrick.xlsx
+++ b/Time Sheet/Patrick.xlsx
@@ -144,26 +144,27 @@
 Added Diagram for project</t>
   </si>
   <si>
+    <t>Updated Project Analysis
+Updated Project Proposal
+Updated sample code for GUI progress table</t>
+  </si>
+  <si>
+    <t>Updated time box items
+Updated logos for splash screen and main app
+Updated sample code which allows disabling of resizing of windows form</t>
+  </si>
+  <si>
+    <t>Week Sunday, 7 August - Saturday, 13 August 2016</t>
+  </si>
+  <si>
     <t>Updated sample code to use threads for background processing
 Updated DSDM methodology 
 Updated Project Diagram
-Added sample GUI with Progres Table</t>
-  </si>
-  <si>
-    <t>Updated Project Analysis
-Updated Project Proposal
-Updated sample code for GUI progress table</t>
-  </si>
-  <si>
-    <t>Updated time box items
-Updated logos for splash screen and main app
-Updated sample code which allows disabling of resizing of windows form</t>
-  </si>
-  <si>
-    <t>Week Sunday, 7 August - Saturday, 13 August 2016</t>
-  </si>
-  <si>
-    <t>Updated time sheet and had project meeting</t>
+Added sample GUI with Progress Table</t>
+  </si>
+  <si>
+    <t>Updated time sheet and had project meeting
+Added sample code for encrypting files</t>
   </si>
 </sst>
 </file>
@@ -554,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +926,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5">
@@ -937,11 +938,11 @@
         <v>8</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -949,7 +950,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5">
@@ -988,12 +989,12 @@
       </c>
       <c r="D45" s="5">
         <f>SUM(D38:D44)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>6</v>
       </c>
@@ -1081,6 +1082,12 @@
         <v>5</v>
       </c>
     </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <f>SUM(D56,D45,D34,D23,D12)</f>
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add some sample code for saving files
</commit_message>
<xml_diff>
--- a/Time Sheet/Patrick.xlsx
+++ b/Time Sheet/Patrick.xlsx
@@ -163,8 +163,9 @@
 Added sample GUI with Progress Table</t>
   </si>
   <si>
-    <t>Updated time sheet and had project meeting
-Added sample code for encrypting files</t>
+    <t xml:space="preserve">Updated time sheet and had project meeting
+Added sample code for encrypting files and saving files
+</t>
   </si>
 </sst>
 </file>
@@ -557,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -1011,7 +1012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
added sample code for getting database list
</commit_message>
<xml_diff>
--- a/Time Sheet/Patrick.xlsx
+++ b/Time Sheet/Patrick.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t xml:space="preserve">Time recorded for: Patrick Cura – Database Evaluator </t>
   </si>
@@ -166,6 +166,11 @@
     <t xml:space="preserve">Updated time sheet and had project meeting
 Added sample code for encrypting files and saving files
 </t>
+  </si>
+  <si>
+    <t>Improved sample code for saving file in any directory
+Created Use Case diagram
+Drafted Activity diagram</t>
   </si>
 </sst>
 </file>
@@ -559,7 +564,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,13 +1029,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
@@ -1038,7 +1047,9 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
@@ -1080,13 +1091,13 @@
       </c>
       <c r="D56" s="5">
         <f>SUM(D49:D55)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D59">
         <f>SUM(D56,D45,D34,D23,D12)</f>
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>